<commit_message>
adding additional Drl input and indicator function
</commit_message>
<xml_diff>
--- a/Docs/Ford Escape Headlamp behavior list.xlsx
+++ b/Docs/Ford Escape Headlamp behavior list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f77d8628ada1f77c/Documents/GitHub Repo/Car LED Controller Project/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{555ECC7D-EE72-42F2-8EB8-A0AA1652F0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90C09C28-7A22-4E22-9FDE-146BE925550B}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{555ECC7D-EE72-42F2-8EB8-A0AA1652F0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{215FEF0F-D387-469D-9FDA-25DA7BC6FFD5}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="32620" windowHeight="21100" xr2:uid="{80A7759D-C5C2-4CFD-B204-4AD675033ADC}"/>
   </bookViews>
@@ -369,23 +369,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -393,6 +384,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -404,13 +404,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,6 +430,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -736,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FBDE48-9E3E-4363-9FB3-60A8643A97EB}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -761,7 +758,7 @@
     <col min="15" max="15" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -782,642 +779,641 @@
       <c r="N1" s="14"/>
       <c r="O1" s="15"/>
     </row>
-    <row r="2" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="10" t="s">
+    <row r="2" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="10" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="9" t="s">
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="N2" s="11"/>
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="18" t="s">
+      <c r="N3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="19" t="s">
+      <c r="O3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="16"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="N4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="O4" s="19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="N5" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" s="19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="N6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="O6" s="19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M7" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="N7" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="O7" s="19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M8" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="N8" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="O8" s="19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M9" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="N9" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="O9" s="19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M10" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="N10" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="O10" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="E10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M11" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="N11" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="O11" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="N12" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="O12" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+      <c r="E12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="N13" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="O13" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="E13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M14" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="N14" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="O14" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="6" t="s">
+      <c r="E14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="M15" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N15" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="O15" s="22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="E15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="30" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N30" t="s">
         <v>28</v>

</xml_diff>